<commit_message>
Update ChanjoKe FHIR IG
</commit_message>
<xml_diff>
--- a/ChanjoKe-FHIR-IG/CodeSystem-KHTS.A.xlsx
+++ b/ChanjoKe-FHIR-IG/CodeSystem-KHTS.A.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://shr.tiberbuapps.com/fhir/CodeSystem/KHTS.A</t>
+    <t>https://intellisoft-consulting.github.io/igs/ChanjoKe-FHIR-IG/CodeSystem/KHTS.A</t>
   </si>
   <si>
     <t>Version</t>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>KHTS.A CodeSystem for Counties in Kenya</t>
+    <t>KenyaCounties CodeSystem for Counties in Kenya</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,19 +60,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-23T12:29:17+03:00</t>
+    <t>2024-08-27T20:30:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>intellisoftkenya</t>
+    <t>Intellisoft Consulting Ltd</t>
   </si>
   <si>
     <t>Contact</t>
   </si>
   <si>
-    <t>intellisoftkenya (http://example.org/example-publisher)</t>
+    <t>Intellisoft Consulting Ltd (https://www.intellisoftkenya.com/, info[at]intellisoftkenya.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CodeSystem for KHTS.A Counties in Kenya</t>
+    <t>CodeSystem for Counties in Kenya</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -138,7 +138,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>mombasa</t>
+    <t>C-001</t>
   </si>
   <si>
     <t>Mombasa</t>
@@ -147,7 +147,7 @@
     <t>County of Residence, Mombasa</t>
   </si>
   <si>
-    <t>kilifi</t>
+    <t>C-002</t>
   </si>
   <si>
     <t>Kilifi</t>
@@ -156,7 +156,7 @@
     <t>County of Residence, Kilifi</t>
   </si>
   <si>
-    <t>tanaRiver</t>
+    <t>C-003</t>
   </si>
   <si>
     <t>Tana River	Hola</t>
@@ -165,7 +165,7 @@
     <t>County of Residence, Tana River	Hola</t>
   </si>
   <si>
-    <t>lamu</t>
+    <t>C-004</t>
   </si>
   <si>
     <t>Lamu</t>

</xml_diff>